<commit_message>
saved the file on the main sheet of the excel
</commit_message>
<xml_diff>
--- a/List of approved Leptospiraceae species.xlsx
+++ b/List of approved Leptospiraceae species.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ltj8\Documents\lepto\pr_lepto\redo_all_pr_lepto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48013B81-EEB0-47CD-B01F-6B464B571C1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D640E281-24DC-4472-8C9C-D855F5C93676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{68749A6A-FAE9-4044-8211-1DD13EADB9DE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{68749A6A-FAE9-4044-8211-1DD13EADB9DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1394,7 +1394,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98C404B9-39FD-4907-9A96-0CE9EC0D86E6}">
   <dimension ref="A1:H91"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>
@@ -3204,7 +3204,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F835F43-B1D9-49EE-89CE-4CCE9EB02998}">
   <dimension ref="A1:H1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:H1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
added the clade Leptospira sanjuanensis belongs to
</commit_message>
<xml_diff>
--- a/List of approved Leptospiraceae species.xlsx
+++ b/List of approved Leptospiraceae species.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ltj8\Documents\lepto\pr_lepto\redo_all_pr_lepto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D640E281-24DC-4472-8C9C-D855F5C93676}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9C3671D-AFEF-4D8E-84AC-1BA42491EC4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{68749A6A-FAE9-4044-8211-1DD13EADB9DE}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{68749A6A-FAE9-4044-8211-1DD13EADB9DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="312">
   <si>
     <t>Nomenclatural status</t>
   </si>
@@ -1394,8 +1394,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98C404B9-39FD-4907-9A96-0CE9EC0D86E6}">
   <dimension ref="A1:H91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H81" sqref="H81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -3115,6 +3115,9 @@
       <c r="F81" s="8" t="s">
         <v>5</v>
       </c>
+      <c r="H81" s="3" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C82" s="6"/>
@@ -3155,7 +3158,7 @@
       </c>
       <c r="H86" s="1">
         <f>COUNTIF(H2:H84, "P1")</f>
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.25">
@@ -3191,7 +3194,7 @@
       </c>
       <c r="H91" s="2">
         <f>SUM(H86:H89)</f>
-        <v>67</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -3205,10 +3208,16 @@
   <dimension ref="A1:H1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
@@ -3238,5 +3247,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>